<commit_message>
fix: updated public database
</commit_message>
<xml_diff>
--- a/import/raw_data/id_action_type.xlsx
+++ b/import/raw_data/id_action_type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bef\GitHub\micat\import\raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenz/Projekte/micat/import/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AAA3EC-6239-4784-A792-B9340D1C6B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439B68BB-2498-5644-B89A-73792AEA5438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40860" yWindow="0" windowWidth="20676" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>id</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>For both electricity and district heat production</t>
+  </si>
+  <si>
+    <t>…</t>
   </si>
 </sst>
 </file>
@@ -243,7 +246,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -259,9 +262,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -299,7 +302,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -405,7 +408,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -555,22 +558,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" customWidth="1"/>
-    <col min="3" max="3" width="79.5546875" customWidth="1"/>
-    <col min="4" max="4" width="25.88671875" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" customWidth="1"/>
+    <col min="3" max="3" width="79.5" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,7 +587,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -598,7 +601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -612,7 +615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -626,7 +629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -640,7 +643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -654,7 +657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -668,7 +671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -682,7 +685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -696,7 +699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>10</v>
       </c>
@@ -710,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>11</v>
       </c>
@@ -724,7 +727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>12</v>
       </c>
@@ -738,7 +741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>13</v>
       </c>
@@ -752,157 +755,168 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>15</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
         <v>17</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>28</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>29</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>31</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>31</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
         <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" t="s">
-        <v>35</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
         <v>34</v>
       </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
         <v>38</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>44</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>45</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <v>1</v>
       </c>
     </row>

</xml_diff>